<commit_message>
change in profit package min and max value
</commit_message>
<xml_diff>
--- a/public/uploads/profit-sample.xlsx
+++ b/public/uploads/profit-sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saim\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hd-v2\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,17 +15,6 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -38,17 +27,17 @@
     <t>cost</t>
   </si>
   <si>
-    <t>profit</t>
+    <t>Selling rates</t>
   </si>
   <si>
-    <t>rates</t>
+    <t>profit percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -59,6 +48,11 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -87,10 +81,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +393,7 @@
   <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,11 +408,11 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1391,7 +1386,7 @@
         <v>225.78</v>
       </c>
       <c r="D66" s="2">
-        <f t="shared" ref="D66:D70" si="2">B66*(C66/100)+B66</f>
+        <f t="shared" ref="D66:D69" si="2">B66*(C66/100)+B66</f>
         <v>371.97560400000003</v>
       </c>
     </row>

</xml_diff>